<commit_message>
Projecto updated. Tirar dúvidas, confirmar o que tá feito e avançar para o packet tracer
</commit_message>
<xml_diff>
--- a/Documentação/Tabelas/Distribuição dos postos de trabalho e equipamentos diversos pelas salas.xlsx
+++ b/Documentação/Tabelas/Distribuição dos postos de trabalho e equipamentos diversos pelas salas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>Sala</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Número de Tomadas Duplas (incluindo folgas)</t>
   </si>
   <si>
-    <t>Número de Portas ligadas aos Switch</t>
-  </si>
-  <si>
     <t>Salas</t>
   </si>
   <si>
@@ -99,31 +96,43 @@
     <t>Impressora(s)</t>
   </si>
   <si>
-    <t>Equipamento</t>
-  </si>
-  <si>
     <t>Número</t>
   </si>
   <si>
-    <t>PCs</t>
-  </si>
-  <si>
     <t>1 Telefone(s)</t>
   </si>
   <si>
     <t>3 Impressora(s)</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=r0dIvaJRjxE</t>
-  </si>
-  <si>
-    <t>https://www.extendoffice.com/documents/excel/2459-excel-sum-cells-with-text-and-numbers.html</t>
-  </si>
-  <si>
-    <t>1 Telefone(s) ?????</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se o telefone for de IP tem que ter uma tomada dupla </t>
+    <t>Foi optado por duplicar o número de tomadas duplas necessárias.</t>
+  </si>
+  <si>
+    <t>Confirmar esta sala.</t>
+  </si>
+  <si>
+    <t>está aqui contabilizado o posto de trabalho que estava na sala de telecomunicações. Confirmar com o stor.</t>
+  </si>
+  <si>
+    <t>Equipamentos</t>
+  </si>
+  <si>
+    <t>PC(s)</t>
+  </si>
+  <si>
+    <t>Número de Portas ligadas aos Switches</t>
+  </si>
+  <si>
+    <t>Tenho 49 Portas ligadas aos switches</t>
+  </si>
+  <si>
+    <t>A mencionar no relatório</t>
+  </si>
+  <si>
+    <t>1 Bastidor / 1 Router / 2 Switches / 1 UPS</t>
+  </si>
+  <si>
+    <t>1 Telefone(s) e 1 Projector</t>
   </si>
 </sst>
 </file>
@@ -184,10 +193,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -221,24 +227,22 @@
   <autoFilter ref="A1:F22"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Número Sala"/>
-    <tableColumn id="2" name="Sala" dataDxfId="5"/>
-    <tableColumn id="6" name="Postos de Trabalho" dataDxfId="4"/>
-    <tableColumn id="7" name="Outros Equipamentos" dataDxfId="3"/>
-    <tableColumn id="8" name="Número de Tomadas Duplas (incluindo folgas)" dataDxfId="2"/>
-    <tableColumn id="9" name="Número de Portas ligadas aos Switch" dataDxfId="1"/>
+    <tableColumn id="2" name="Sala" dataDxfId="4"/>
+    <tableColumn id="6" name="Postos de Trabalho" dataDxfId="3"/>
+    <tableColumn id="7" name="Outros Equipamentos" dataDxfId="2"/>
+    <tableColumn id="8" name="Número de Tomadas Duplas (incluindo folgas)" dataDxfId="1"/>
+    <tableColumn id="9" name="Número de Portas ligadas aos Switches" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="I1:J4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="I1:J4" totalsRowShown="0">
   <autoFilter ref="I1:J4"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Equipamento"/>
-    <tableColumn id="2" name="Número" dataDxfId="0">
-      <calculatedColumnFormula>SUM(IF(ISNUMBER(FIND(I2,D2:D21)),VALUE(LEFT(D2:D21,(FIND(I2,D2:D21)-1)))))</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" name="Equipamentos"/>
+    <tableColumn id="2" name="Número"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -543,25 +547,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" customWidth="1"/>
     <col min="3" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" customWidth="1"/>
     <col min="6" max="6" width="34.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -576,13 +582,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -590,22 +596,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="J2">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -613,26 +622,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J4" si="0">SUM(IF(ISNUMBER(FIND(I3,D3:D22)),VALUE(LEFT(D3:D22,(FIND(I3,D3:D22)-1)))))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -640,26 +648,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -667,19 +674,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -687,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -696,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3">
         <v>1</v>
@@ -707,19 +714,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3">
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F7" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -727,19 +734,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -747,19 +754,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -767,19 +774,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -787,19 +794,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -807,19 +814,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -827,19 +834,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -847,19 +854,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3">
         <v>3</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -867,19 +874,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E15" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15" s="3">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -887,19 +897,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3">
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F16" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -907,19 +917,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="3">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -927,22 +940,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E18" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -950,19 +960,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -970,7 +980,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -983,6 +993,9 @@
       </c>
       <c r="F20" s="3">
         <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -990,16 +1003,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E21" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F21" s="3">
         <v>3</v>
@@ -1007,7 +1020,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3">
@@ -1015,29 +1028,26 @@
         <v>30</v>
       </c>
       <c r="D22" s="3">
-        <v>20</v>
+        <f>SUM(J2:J3)</f>
+        <v>19</v>
       </c>
       <c r="E22" s="3">
         <f>SUM(E2:E21)</f>
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="F22" s="3">
         <f>SUM(F2:F21)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D28" t="e">
-        <f>SUM(IF((RIGHT(D2:D21,1))=I2,(--LEFT((SUM(D2:D21="",0,D2:D21)),2)),0))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E29" t="s">
-        <v>30</v>
+      <c r="A28" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -1292,78 +1302,78 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>